<commit_message>
Booking Engine Code updated in TestBase
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Admin_Data.xlsx
+++ b/src/test/resources/testData/Admin_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="395">
   <si>
     <t>Username</t>
   </si>
@@ -314,12 +314,6 @@
     <t>Rateplan2</t>
   </si>
   <si>
-    <t>01-20-22</t>
-  </si>
-  <si>
-    <t>01-21-22</t>
-  </si>
-  <si>
     <t>200</t>
   </si>
   <si>
@@ -341,15 +335,6 @@
     <t>ConfirmationNo</t>
   </si>
   <si>
-    <t>12-01-21</t>
-  </si>
-  <si>
-    <t>12-30-21</t>
-  </si>
-  <si>
-    <t>ALH100001888</t>
-  </si>
-  <si>
     <t>BrandName</t>
   </si>
   <si>
@@ -1203,6 +1188,48 @@
   </si>
   <si>
     <t>RoomNameTextbox</t>
+  </si>
+  <si>
+    <t>gdsCode</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>ghi</t>
+  </si>
+  <si>
+    <t>jkl</t>
+  </si>
+  <si>
+    <t>mno</t>
+  </si>
+  <si>
+    <t>pqr</t>
+  </si>
+  <si>
+    <t>stu</t>
+  </si>
+  <si>
+    <t>vwx</t>
+  </si>
+  <si>
+    <t>01-28-22</t>
+  </si>
+  <si>
+    <t>01-25-22</t>
+  </si>
+  <si>
+    <t>02-20-22</t>
+  </si>
+  <si>
+    <t>02-24-22</t>
+  </si>
+  <si>
+    <t>ALH100001928</t>
   </si>
 </sst>
 </file>
@@ -1582,22 +1609,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" t="s">
         <v>139</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1608,22 +1635,22 @@
         <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1748,7 +1775,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,25 +1810,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1825,8 +1852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,24 +1863,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
         <v>95</v>
-      </c>
-      <c r="B1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>98</v>
+        <v>391</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>99</v>
+        <v>390</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>100</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -1863,10 +1890,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AB10"/>
   <sheetViews>
     <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,11 +1919,12 @@
     <col min="23" max="23" width="18.140625" customWidth="1"/>
     <col min="24" max="24" width="17.42578125" customWidth="1"/>
     <col min="25" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.5703125" customWidth="1"/>
-    <col min="27" max="27" width="15.85546875" customWidth="1"/>
+    <col min="26" max="26" width="10.28515625" customWidth="1"/>
+    <col min="27" max="27" width="14.5703125" customWidth="1"/>
+    <col min="28" max="28" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1904,117 +1932,120 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" t="s">
         <v>151</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>152</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>153</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>154</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>157</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>158</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>159</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>160</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>161</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>162</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>163</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>164</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
         <v>165</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
         <v>166</v>
       </c>
-      <c r="S1" t="s">
+      <c r="X1" t="s">
         <v>167</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
         <v>168</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Z1" t="s">
+        <v>381</v>
+      </c>
+      <c r="AA1" t="s">
         <v>169</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AB1" t="s">
         <v>170</v>
       </c>
-      <c r="W1" t="s">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>171</v>
       </c>
-      <c r="X1" t="s">
+      <c r="B2" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" t="s">
         <v>173</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="E2" t="s">
         <v>174</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="F2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G2" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="H2" t="s">
         <v>177</v>
-      </c>
-      <c r="C2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F2" t="s">
-        <v>180</v>
-      </c>
-      <c r="G2" t="s">
-        <v>181</v>
-      </c>
-      <c r="H2" t="s">
-        <v>182</v>
       </c>
       <c r="I2">
         <v>411057</v>
       </c>
       <c r="J2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="K2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="L2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="M2">
         <v>99349011</v>
@@ -2023,7 +2054,7 @@
         <v>402971</v>
       </c>
       <c r="O2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -2032,7 +2063,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="S2" s="7">
         <v>44847</v>
@@ -2041,51 +2072,54 @@
         <v>44909</v>
       </c>
       <c r="U2" t="s">
+        <v>182</v>
+      </c>
+      <c r="V2" t="s">
+        <v>183</v>
+      </c>
+      <c r="W2" t="s">
+        <v>184</v>
+      </c>
+      <c r="X2" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>382</v>
+      </c>
+      <c r="AA2" t="s">
         <v>187</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AB2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>188</v>
       </c>
-      <c r="W2" t="s">
+      <c r="E3" t="s">
         <v>189</v>
       </c>
-      <c r="X2" t="s">
+      <c r="F3" t="s">
         <v>190</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="K3" t="s">
         <v>191</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="L3" t="s">
         <v>192</v>
       </c>
-      <c r="AA2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="M3" t="s">
         <v>193</v>
       </c>
-      <c r="E3" t="s">
+      <c r="N3" t="s">
         <v>194</v>
       </c>
-      <c r="F3" t="s">
+      <c r="O3" t="s">
         <v>195</v>
-      </c>
-      <c r="K3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L3" t="s">
-        <v>197</v>
-      </c>
-      <c r="M3" t="s">
-        <v>198</v>
-      </c>
-      <c r="N3" t="s">
-        <v>199</v>
-      </c>
-      <c r="O3" t="s">
-        <v>200</v>
       </c>
       <c r="P3">
         <v>10000</v>
@@ -2097,117 +2131,138 @@
         <v>44910</v>
       </c>
       <c r="U3" t="s">
+        <v>196</v>
+      </c>
+      <c r="X3" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>383</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
         <v>201</v>
       </c>
-      <c r="X3" t="s">
+      <c r="L4" t="s">
         <v>202</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="O4" t="s">
         <v>203</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="X4" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y4" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="Z4" t="s">
+        <v>384</v>
+      </c>
+      <c r="AB4" t="s">
         <v>205</v>
       </c>
-      <c r="K4" t="s">
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>206</v>
       </c>
-      <c r="L4" t="s">
+      <c r="E5" t="s">
         <v>207</v>
       </c>
-      <c r="O4" t="s">
+      <c r="K5" t="s">
         <v>208</v>
       </c>
-      <c r="X4" t="s">
-        <v>201</v>
-      </c>
-      <c r="Y4" t="s">
+      <c r="L5" t="s">
         <v>209</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="X5" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="Y5" t="s">
         <v>211</v>
       </c>
-      <c r="E5" t="s">
+      <c r="Z5" t="s">
+        <v>385</v>
+      </c>
+      <c r="AB5" t="s">
         <v>212</v>
       </c>
-      <c r="K5" t="s">
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>213</v>
       </c>
-      <c r="L5" t="s">
+      <c r="E6" t="s">
         <v>214</v>
       </c>
-      <c r="X5" t="s">
+      <c r="K6" t="s">
         <v>215</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="X6" t="s">
         <v>216</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="Y6" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="Z6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
         <v>218</v>
       </c>
-      <c r="E6" t="s">
+      <c r="X7" t="s">
         <v>219</v>
       </c>
-      <c r="K6" t="s">
+      <c r="Y7" t="s">
         <v>220</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Z7" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X8" t="s">
         <v>221</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Y8" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
+      <c r="Z8" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X9" t="s">
         <v>223</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y9" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>215</v>
+      </c>
+      <c r="Y10" t="s">
         <v>224</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="X8" t="s">
-        <v>226</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="X9" t="s">
-        <v>228</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>220</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2234,75 +2289,75 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" t="s">
         <v>230</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>231</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>232</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>233</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>234</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>235</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>236</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>237</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>238</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>239</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>240</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>241</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>242</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>243</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>244</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>245</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>246</v>
-      </c>
-      <c r="R1" t="s">
-        <v>247</v>
-      </c>
-      <c r="S1" t="s">
-        <v>248</v>
-      </c>
-      <c r="T1" t="s">
-        <v>249</v>
-      </c>
-      <c r="U1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C2" s="11">
         <v>200</v>
@@ -2311,7 +2366,7 @@
         <v>1000</v>
       </c>
       <c r="E2" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F2" s="11">
         <v>200</v>
@@ -2320,10 +2375,10 @@
         <v>2000</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="I2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J2" s="11">
         <v>200</v>
@@ -2332,10 +2387,10 @@
         <v>3000</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="M2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="N2" s="11">
         <v>200</v>
@@ -2344,22 +2399,22 @@
         <v>4000</v>
       </c>
       <c r="P2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="Q2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="R2" s="11">
         <v>500</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="U2" s="14" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="W2" s="11"/>
       <c r="X2" s="11"/>
@@ -2394,96 +2449,96 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" t="s">
         <v>261</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>262</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>263</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>264</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>265</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>266</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>267</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>268</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>269</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>270</v>
-      </c>
-      <c r="K1" t="s">
-        <v>271</v>
-      </c>
-      <c r="L1" t="s">
-        <v>272</v>
-      </c>
-      <c r="M1" t="s">
-        <v>273</v>
-      </c>
-      <c r="N1" t="s">
-        <v>274</v>
-      </c>
-      <c r="O1" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C2">
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="F2">
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="H2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I2">
         <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="K2" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="L2">
         <v>5</v>
       </c>
       <c r="M2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="N2">
         <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2512,60 +2567,60 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="F1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="G1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="I1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B2" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="E2">
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="G2" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="H2">
         <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2599,75 +2654,75 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H1" t="s">
         <v>263</v>
       </c>
-      <c r="D1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E1" t="s">
-        <v>265</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>264</v>
+      </c>
+      <c r="J1" t="s">
+        <v>289</v>
+      </c>
+      <c r="K1" t="s">
         <v>266</v>
       </c>
-      <c r="G1" t="s">
-        <v>293</v>
-      </c>
-      <c r="H1" t="s">
-        <v>268</v>
-      </c>
-      <c r="I1" t="s">
-        <v>269</v>
-      </c>
-      <c r="J1" t="s">
-        <v>294</v>
-      </c>
-      <c r="K1" t="s">
-        <v>271</v>
-      </c>
       <c r="L1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C2">
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E2" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="H2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I2">
         <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="K2" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="L2">
         <v>18</v>
@@ -2699,66 +2754,66 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I1" t="s">
+        <v>301</v>
+      </c>
+      <c r="J1" t="s">
         <v>302</v>
-      </c>
-      <c r="B1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D1" t="s">
-        <v>303</v>
-      </c>
-      <c r="E1" t="s">
-        <v>231</v>
-      </c>
-      <c r="F1" t="s">
-        <v>286</v>
-      </c>
-      <c r="G1" t="s">
-        <v>304</v>
-      </c>
-      <c r="H1" t="s">
-        <v>305</v>
-      </c>
-      <c r="I1" t="s">
-        <v>306</v>
-      </c>
-      <c r="J1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B2" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C2">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E2" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="F2">
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="H2" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I2">
         <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -2788,84 +2843,84 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D1" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="G1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="I1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="J1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="K1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="L1" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="M1" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C2">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="F2">
         <v>9</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="I2">
         <v>11</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="L2">
         <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -2885,18 +2940,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2929,78 +2984,78 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F1" t="s">
         <v>326</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>327</v>
       </c>
-      <c r="C1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D1" t="s">
-        <v>329</v>
-      </c>
-      <c r="E1" t="s">
-        <v>330</v>
-      </c>
-      <c r="F1" t="s">
-        <v>331</v>
-      </c>
-      <c r="G1" t="s">
-        <v>332</v>
-      </c>
       <c r="H1" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="I1" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="J1" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="K1" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="L1" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B2" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="E2" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F2" s="2">
         <v>30</v>
       </c>
       <c r="G2" t="s">
+        <v>371</v>
+      </c>
+      <c r="H2" t="s">
+        <v>372</v>
+      </c>
+      <c r="I2" t="s">
+        <v>373</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="L2" t="s">
         <v>376</v>
-      </c>
-      <c r="H2" t="s">
-        <v>377</v>
-      </c>
-      <c r="I2" t="s">
-        <v>378</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="L2" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3032,57 +3087,57 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D1" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="E1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="G1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="H1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B2" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="E2" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="H2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="I2">
         <v>3</v>
@@ -3105,72 +3160,72 @@
   <sheetData>
     <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="F1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G1" t="s">
+        <v>344</v>
+      </c>
+      <c r="H1" t="s">
         <v>345</v>
       </c>
-      <c r="B1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="I1" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
+        <v>263</v>
+      </c>
+      <c r="K1" t="s">
         <v>347</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="L1" t="s">
         <v>348</v>
       </c>
-      <c r="F1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="M1" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
+        <v>266</v>
+      </c>
+      <c r="O1" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="P1" t="s">
         <v>351</v>
       </c>
-      <c r="J1" t="s">
-        <v>268</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="Q1" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
+        <v>270</v>
+      </c>
+      <c r="S1" t="s">
         <v>353</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="T1" t="s">
         <v>354</v>
-      </c>
-      <c r="N1" t="s">
-        <v>271</v>
-      </c>
-      <c r="O1" t="s">
-        <v>355</v>
-      </c>
-      <c r="P1" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="R1" t="s">
-        <v>275</v>
-      </c>
-      <c r="S1" t="s">
-        <v>358</v>
-      </c>
-      <c r="T1" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C2" s="11">
         <v>800</v>
@@ -3179,10 +3234,10 @@
         <v>800</v>
       </c>
       <c r="E2" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="F2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G2" s="11">
         <v>200</v>
@@ -3191,10 +3246,10 @@
         <v>1300</v>
       </c>
       <c r="I2" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="J2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="K2" s="11">
         <v>200</v>
@@ -3203,10 +3258,10 @@
         <v>1000</v>
       </c>
       <c r="M2" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="N2" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="O2" s="11">
         <v>200</v>
@@ -3215,10 +3270,10 @@
         <v>1000</v>
       </c>
       <c r="Q2" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="R2" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="S2" s="11">
         <v>200</v>
@@ -3260,90 +3315,90 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>106</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>107</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>109</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>110</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>111</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>112</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>113</v>
-      </c>
-      <c r="J1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K1" t="s">
-        <v>115</v>
-      </c>
-      <c r="L1" t="s">
-        <v>116</v>
-      </c>
-      <c r="M1" t="s">
-        <v>117</v>
-      </c>
-      <c r="N1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B2" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C2" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J2" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="K2" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="M2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N2" t="s">
         <v>123</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="J2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="N2" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3366,36 +3421,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -3495,7 +3550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -3512,7 +3567,7 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Call centre Booking Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Admin_Data.xlsx
+++ b/src/test/resources/testData/Admin_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="25" activeTab="30"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="26" activeTab="31"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -43,8 +43,9 @@
     <sheet name="PropertyRestriction" sheetId="33" r:id="rId29"/>
     <sheet name="SmartRate" sheetId="34" r:id="rId30"/>
     <sheet name="CompoundAccessCode" sheetId="35" r:id="rId31"/>
+    <sheet name="Booking" sheetId="36" r:id="rId32"/>
   </sheets>
-  <calcPr calcId="0" concurrentManualCount="2"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="466">
   <si>
     <t>Username</t>
   </si>
@@ -1428,6 +1429,30 @@
   </si>
   <si>
     <t>CAC2022</t>
+  </si>
+  <si>
+    <t>ArrivalD</t>
+  </si>
+  <si>
+    <t>DepartureD</t>
+  </si>
+  <si>
+    <t>AccessCode2</t>
+  </si>
+  <si>
+    <t>Summer Special -SS</t>
+  </si>
+  <si>
+    <t>AC1</t>
+  </si>
+  <si>
+    <t>02/10/2022</t>
+  </si>
+  <si>
+    <t>02/12/2022</t>
+  </si>
+  <si>
+    <t>AC1Edit</t>
   </si>
 </sst>
 </file>
@@ -4315,7 +4340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -4329,6 +4354,62 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>457</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D1" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B2" t="s">
+        <v>462</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="E2" t="s">
+        <v>465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mobile Booking code Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Admin_Data.xlsx
+++ b/src/test/resources/testData/Admin_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="29" activeTab="33"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="30" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -46,6 +46,7 @@
     <sheet name="Booking" sheetId="36" r:id="rId32"/>
     <sheet name="NormalSingleRoomBookingData" sheetId="37" r:id="rId33"/>
     <sheet name="MobileB" sheetId="38" r:id="rId34"/>
+    <sheet name="Sheet2" sheetId="39" r:id="rId35"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="504">
   <si>
     <t>Username</t>
   </si>
@@ -1520,13 +1521,55 @@
     <t>CCode</t>
   </si>
   <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Dk</t>
+  </si>
+  <si>
+    <t>7883664742</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>600064</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>4012 8888 8888 1881</t>
+  </si>
+  <si>
+    <t>11/22</t>
+  </si>
+  <si>
     <t>AnkitaM</t>
   </si>
   <si>
     <t>ankita.mohamanasingh@pegs.com</t>
   </si>
   <si>
-    <t>5454545454545454</t>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>5454</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>28</t>
   </si>
 </sst>
 </file>
@@ -1583,7 +1626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1603,6 +1646,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4662,20 +4706,21 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>482</v>
       </c>
@@ -4706,16 +4751,19 @@
       <c r="J1" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>487</v>
-      </c>
-      <c r="B2">
-        <v>123456789</v>
+        <v>497</v>
+      </c>
+      <c r="B2" t="s">
+        <v>499</v>
       </c>
       <c r="C2" t="s">
-        <v>488</v>
+        <v>498</v>
       </c>
       <c r="D2" t="s">
         <v>414</v>
@@ -4726,17 +4774,130 @@
       <c r="F2" t="s">
         <v>414</v>
       </c>
-      <c r="G2">
-        <v>123456</v>
+      <c r="G2" s="3" t="s">
+        <v>500</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H4" s="3" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H5" s="3" t="s">
+        <v>501</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" t="s">
+        <v>487</v>
+      </c>
+      <c r="F1" t="s">
+        <v>483</v>
+      </c>
+      <c r="G1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" t="s">
+        <v>437</v>
+      </c>
+      <c r="I1" t="s">
+        <v>484</v>
+      </c>
+      <c r="J1" t="s">
+        <v>485</v>
+      </c>
+      <c r="K1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>489</v>
       </c>
-      <c r="I2">
-        <v>1112</v>
-      </c>
-      <c r="J2">
-        <v>123</v>
+      <c r="B2" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="C2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" t="s">
+        <v>491</v>
+      </c>
+      <c r="E2" t="s">
+        <v>488</v>
+      </c>
+      <c r="F2" t="s">
+        <v>492</v>
+      </c>
+      <c r="G2" t="s">
+        <v>491</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Call Center Booking Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Admin_Data.xlsx
+++ b/src/test/resources/testData/Admin_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="30" activeTab="33"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="34" activeTab="37"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,10 @@
     <sheet name="Booking" sheetId="36" r:id="rId32"/>
     <sheet name="NormalSingleRoomBookingData" sheetId="37" r:id="rId33"/>
     <sheet name="MobileB" sheetId="38" r:id="rId34"/>
-    <sheet name="Sheet2" sheetId="39" r:id="rId35"/>
+    <sheet name="ModifyingReservation" sheetId="40" r:id="rId35"/>
+    <sheet name="DynamicPricingRule" sheetId="41" r:id="rId36"/>
+    <sheet name="CalendarViewBooking" sheetId="42" r:id="rId37"/>
+    <sheet name="GroupBlockBooking" sheetId="43" r:id="rId38"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -58,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="544">
   <si>
     <t>Username</t>
   </si>
@@ -1527,30 +1530,6 @@
     <t>India</t>
   </si>
   <si>
-    <t>Dk</t>
-  </si>
-  <si>
-    <t>7883664742</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>Tamil Nadu</t>
-  </si>
-  <si>
-    <t>600064</t>
-  </si>
-  <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>4012 8888 8888 1881</t>
-  </si>
-  <si>
-    <t>11/22</t>
-  </si>
-  <si>
     <t>AnkitaM</t>
   </si>
   <si>
@@ -1570,6 +1549,152 @@
   </si>
   <si>
     <t>28</t>
+  </si>
+  <si>
+    <t>AmountBeforeAddTaxTc_01</t>
+  </si>
+  <si>
+    <t>AmountAfterAddTaxTc_01</t>
+  </si>
+  <si>
+    <t>AmountBeforeAddTaxTc_02</t>
+  </si>
+  <si>
+    <t>AmountAfterAddTaxTc_02</t>
+  </si>
+  <si>
+    <t>AmountBeforeAddTaxTc_03</t>
+  </si>
+  <si>
+    <t>AmountAfterAddTaxTc_03</t>
+  </si>
+  <si>
+    <t>ConfirmCode</t>
+  </si>
+  <si>
+    <t>GuestDetailBefore</t>
+  </si>
+  <si>
+    <t>GuestDetailAfter</t>
+  </si>
+  <si>
+    <t>USD 0.00</t>
+  </si>
+  <si>
+    <t>USD 45.00</t>
+  </si>
+  <si>
+    <t>USD 22.50</t>
+  </si>
+  <si>
+    <t>MH100003632</t>
+  </si>
+  <si>
+    <t>Sudhakar Mourya
+sudhakar.mourya@igtsolutions.com</t>
+  </si>
+  <si>
+    <t>Rohan Sharma
+sudhakar.mourya@igtsolutions.com</t>
+  </si>
+  <si>
+    <t>Rohan</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>sudhakar.mourya@igtsolutions.com</t>
+  </si>
+  <si>
+    <t>233</t>
+  </si>
+  <si>
+    <t>ruleName</t>
+  </si>
+  <si>
+    <t>ruleCode</t>
+  </si>
+  <si>
+    <t>shortDescription</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>First Few Nights</t>
+  </si>
+  <si>
+    <t>FFN</t>
+  </si>
+  <si>
+    <t>Exciting Plan</t>
+  </si>
+  <si>
+    <t>Future Price</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>Latest Plan</t>
+  </si>
+  <si>
+    <t>Diwali Offer</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>Regular Offer</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>subdomain</t>
+  </si>
+  <si>
+    <t>admin@traveltripper.com</t>
+  </si>
+  <si>
+    <t>bookingissoeasy</t>
+  </si>
+  <si>
+    <t>ostwal</t>
+  </si>
+  <si>
+    <t>Sudhakar</t>
+  </si>
+  <si>
+    <t>Mourya</t>
+  </si>
+  <si>
+    <t>sudhakar cc</t>
+  </si>
+  <si>
+    <t>NameRatePlan</t>
+  </si>
+  <si>
+    <t>RateTypeCode</t>
+  </si>
+  <si>
+    <t>Diwali Rate Plan</t>
+  </si>
+  <si>
+    <t>DPR</t>
+  </si>
+  <si>
+    <t>DRP</t>
+  </si>
+  <si>
+    <t>Diwali Plan</t>
+  </si>
+  <si>
+    <t>DDL</t>
   </si>
 </sst>
 </file>
@@ -1626,7 +1751,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1646,7 +1771,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1928,10 +2052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I1" sqref="I1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1942,10 +2066,11 @@
     <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1970,8 +2095,35 @@
       <c r="H1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>496</v>
+      </c>
+      <c r="J1" t="s">
+        <v>497</v>
+      </c>
+      <c r="K1" t="s">
+        <v>498</v>
+      </c>
+      <c r="L1" t="s">
+        <v>499</v>
+      </c>
+      <c r="M1" t="s">
+        <v>500</v>
+      </c>
+      <c r="N1" t="s">
+        <v>501</v>
+      </c>
+      <c r="O1" t="s">
+        <v>502</v>
+      </c>
+      <c r="P1" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
@@ -1995,6 +2147,33 @@
       </c>
       <c r="H2" s="10" t="s">
         <v>143</v>
+      </c>
+      <c r="I2" t="s">
+        <v>505</v>
+      </c>
+      <c r="J2" t="s">
+        <v>506</v>
+      </c>
+      <c r="K2" t="s">
+        <v>506</v>
+      </c>
+      <c r="L2" t="s">
+        <v>505</v>
+      </c>
+      <c r="M2" t="s">
+        <v>506</v>
+      </c>
+      <c r="N2" t="s">
+        <v>507</v>
+      </c>
+      <c r="O2" t="s">
+        <v>508</v>
+      </c>
+      <c r="P2" t="s">
+        <v>509</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>510</v>
       </c>
     </row>
   </sheetData>
@@ -4708,7 +4887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -4757,13 +4936,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="B2" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="C2" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="D2" t="s">
         <v>414</v>
@@ -4775,13 +4954,13 @@
         <v>414</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>133</v>
@@ -4792,20 +4971,20 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H3" s="3" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H4" s="3" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H5" s="3" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -4816,88 +4995,355 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>482</v>
+        <v>396</v>
       </c>
       <c r="B1" t="s">
-        <v>436</v>
+        <v>397</v>
       </c>
       <c r="C1" t="s">
         <v>398</v>
       </c>
       <c r="D1" t="s">
-        <v>151</v>
+        <v>403</v>
       </c>
       <c r="E1" t="s">
-        <v>487</v>
+        <v>404</v>
       </c>
       <c r="F1" t="s">
-        <v>483</v>
+        <v>405</v>
       </c>
       <c r="G1" t="s">
+        <v>406</v>
+      </c>
+      <c r="H1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>511</v>
+      </c>
+      <c r="B2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C2" t="s">
+        <v>513</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>514</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B1" t="s">
+        <v>516</v>
+      </c>
+      <c r="C1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>519</v>
+      </c>
+      <c r="B2" t="s">
+        <v>520</v>
+      </c>
+      <c r="C2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>522</v>
+      </c>
+      <c r="B3" t="s">
+        <v>523</v>
+      </c>
+      <c r="C3" t="s">
+        <v>524</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>525</v>
+      </c>
+      <c r="B4" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>527</v>
+      </c>
+      <c r="B5" t="s">
+        <v>520</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
+        <v>396</v>
+      </c>
+      <c r="F1" t="s">
+        <v>397</v>
+      </c>
+      <c r="G1" t="s">
+        <v>398</v>
+      </c>
+      <c r="H1" t="s">
+        <v>399</v>
+      </c>
+      <c r="I1" t="s">
+        <v>400</v>
+      </c>
+      <c r="J1" t="s">
         <v>104</v>
       </c>
-      <c r="H1" t="s">
-        <v>437</v>
-      </c>
-      <c r="I1" t="s">
-        <v>484</v>
-      </c>
-      <c r="J1" t="s">
-        <v>485</v>
-      </c>
       <c r="K1" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="L1" t="s">
+        <v>401</v>
+      </c>
+      <c r="M1" t="s">
+        <v>402</v>
+      </c>
+      <c r="N1" t="s">
+        <v>403</v>
+      </c>
+      <c r="O1" t="s">
+        <v>404</v>
+      </c>
+      <c r="P1" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>489</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>490</v>
+        <v>531</v>
+      </c>
+      <c r="B2" t="s">
+        <v>532</v>
       </c>
       <c r="C2" t="s">
-        <v>145</v>
+        <v>533</v>
       </c>
       <c r="D2" t="s">
-        <v>491</v>
+        <v>142</v>
       </c>
       <c r="E2" t="s">
-        <v>488</v>
+        <v>534</v>
       </c>
       <c r="F2" t="s">
-        <v>492</v>
+        <v>535</v>
       </c>
       <c r="G2" t="s">
-        <v>491</v>
+        <v>513</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>493</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>496</v>
+        <v>133</v>
+      </c>
+      <c r="I2" t="s">
+        <v>414</v>
+      </c>
+      <c r="J2" t="s">
+        <v>414</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>494</v>
+        <v>415</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="M2" t="s">
+        <v>536</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N3" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1" t="s">
+        <v>537</v>
+      </c>
+      <c r="E1" t="s">
+        <v>538</v>
+      </c>
+      <c r="F1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>539</v>
+      </c>
+      <c r="B2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>539</v>
+      </c>
+      <c r="E2" t="s">
+        <v>541</v>
+      </c>
+      <c r="F2" t="s">
+        <v>542</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Admin and Callcenter Codes are updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Admin_Data.xlsx
+++ b/src/test/resources/testData/Admin_Data.xlsx
@@ -3,51 +3,57 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fw\NewFramework\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="2715" firstSheet="31" activeTab="33"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="2715"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
-    <sheet name="Brand" sheetId="10" r:id="rId2"/>
-    <sheet name="Property" sheetId="11" r:id="rId3"/>
-    <sheet name="Channel" sheetId="12" r:id="rId4"/>
-    <sheet name="GuestPrefQuesData" sheetId="2" r:id="rId5"/>
-    <sheet name="RatePlanPageData" sheetId="26" r:id="rId6"/>
-    <sheet name="AddOnsData" sheetId="3" r:id="rId7"/>
-    <sheet name="RatePlanCategoriesData" sheetId="4" r:id="rId8"/>
-    <sheet name="SmartPoliciesData" sheetId="5" r:id="rId9"/>
-    <sheet name="AddOrDeltePolicyData" sheetId="6" r:id="rId10"/>
-    <sheet name="RateGrid" sheetId="8" r:id="rId11"/>
-    <sheet name="Reports" sheetId="9" r:id="rId12"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId13"/>
-    <sheet name="MeetingRoom2" sheetId="15" r:id="rId14"/>
-    <sheet name="Dining" sheetId="16" r:id="rId15"/>
-    <sheet name="Dining2" sheetId="17" r:id="rId16"/>
-    <sheet name="Airport1" sheetId="18" r:id="rId17"/>
-    <sheet name="Airport2" sheetId="19" r:id="rId18"/>
-    <sheet name="Attraction2" sheetId="25" r:id="rId19"/>
-    <sheet name="Taxes" sheetId="24" r:id="rId20"/>
-    <sheet name="Attraction" sheetId="22" r:id="rId21"/>
-    <sheet name="MeetingRoomMR" sheetId="23" r:id="rId22"/>
-    <sheet name="JCCBookings" sheetId="27" r:id="rId23"/>
-    <sheet name="HouseInventoryRestrictions" sheetId="28" r:id="rId24"/>
-    <sheet name="URLPB1" sheetId="29" r:id="rId25"/>
-    <sheet name="URLPB2" sheetId="30" r:id="rId26"/>
-    <sheet name="URLPB3" sheetId="31" r:id="rId27"/>
-    <sheet name="URLPB4" sheetId="32" r:id="rId28"/>
-    <sheet name="PropertyRestriction" sheetId="33" r:id="rId29"/>
-    <sheet name="SmartRate" sheetId="34" r:id="rId30"/>
-    <sheet name="CompoundAccessCode" sheetId="35" r:id="rId31"/>
-    <sheet name="Booking" sheetId="36" r:id="rId32"/>
-    <sheet name="NormalSingleRoomBookingData" sheetId="37" r:id="rId33"/>
-    <sheet name="MobileB" sheetId="38" r:id="rId34"/>
-    <sheet name="ModifyingReservation" sheetId="40" r:id="rId35"/>
-    <sheet name="DynamicPricingRule" sheetId="41" r:id="rId36"/>
-    <sheet name="CalendarViewBooking" sheetId="42" r:id="rId37"/>
-    <sheet name="GroupBlockBooking" sheetId="43" r:id="rId38"/>
+    <sheet name="ACB" sheetId="44" r:id="rId2"/>
+    <sheet name="Brand" sheetId="10" r:id="rId3"/>
+    <sheet name="Property" sheetId="11" r:id="rId4"/>
+    <sheet name="Channel" sheetId="12" r:id="rId5"/>
+    <sheet name="GuestPrefQuesData" sheetId="2" r:id="rId6"/>
+    <sheet name="RatePlanPageData" sheetId="26" r:id="rId7"/>
+    <sheet name="AddOnsData" sheetId="3" r:id="rId8"/>
+    <sheet name="RatePlanCategoriesData" sheetId="4" r:id="rId9"/>
+    <sheet name="SmartPoliciesData" sheetId="5" r:id="rId10"/>
+    <sheet name="AddOrDeltePolicyData" sheetId="6" r:id="rId11"/>
+    <sheet name="RateGrid" sheetId="8" r:id="rId12"/>
+    <sheet name="Reports" sheetId="9" r:id="rId13"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId14"/>
+    <sheet name="MeetingRoom2" sheetId="15" r:id="rId15"/>
+    <sheet name="Dining" sheetId="16" r:id="rId16"/>
+    <sheet name="Dining2" sheetId="17" r:id="rId17"/>
+    <sheet name="Airport1" sheetId="18" r:id="rId18"/>
+    <sheet name="Airport2" sheetId="19" r:id="rId19"/>
+    <sheet name="Attraction2" sheetId="25" r:id="rId20"/>
+    <sheet name="Taxes" sheetId="24" r:id="rId21"/>
+    <sheet name="Attraction" sheetId="22" r:id="rId22"/>
+    <sheet name="MeetingRoomMR" sheetId="23" r:id="rId23"/>
+    <sheet name="JCCBookings" sheetId="27" r:id="rId24"/>
+    <sheet name="HouseInventoryRestrictions" sheetId="28" r:id="rId25"/>
+    <sheet name="URLPB1" sheetId="29" r:id="rId26"/>
+    <sheet name="URLPB2" sheetId="30" r:id="rId27"/>
+    <sheet name="URLPB3" sheetId="31" r:id="rId28"/>
+    <sheet name="URLPB4" sheetId="32" r:id="rId29"/>
+    <sheet name="PropertyRestriction" sheetId="33" r:id="rId30"/>
+    <sheet name="SmartRate" sheetId="34" r:id="rId31"/>
+    <sheet name="CompoundAccessCode" sheetId="35" r:id="rId32"/>
+    <sheet name="Booking" sheetId="36" r:id="rId33"/>
+    <sheet name="NormalSingleRoomBookingData" sheetId="37" r:id="rId34"/>
+    <sheet name="MobileB" sheetId="38" r:id="rId35"/>
+    <sheet name="MBTC7" sheetId="45" r:id="rId36"/>
+    <sheet name="ModifyingReservation" sheetId="40" r:id="rId37"/>
+    <sheet name="DynamicPricingRule" sheetId="41" r:id="rId38"/>
+    <sheet name="CalendarViewBooking" sheetId="42" r:id="rId39"/>
+    <sheet name="GroupBlockBooking" sheetId="43" r:id="rId40"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="554">
   <si>
     <t>Username</t>
   </si>
@@ -1697,6 +1703,30 @@
   </si>
   <si>
     <t>'5454</t>
+  </si>
+  <si>
+    <t>SummerSpecial -SS</t>
+  </si>
+  <si>
+    <t>02/25/2022</t>
+  </si>
+  <si>
+    <t>02/28/2022</t>
+  </si>
+  <si>
+    <t>WebConfirmMailId</t>
+  </si>
+  <si>
+    <t>WebConfirmCode</t>
+  </si>
+  <si>
+    <t>MobConfirmCode</t>
+  </si>
+  <si>
+    <t>MobConfirmMailId</t>
+  </si>
+  <si>
+    <t>MH100004181</t>
   </si>
 </sst>
 </file>
@@ -2054,10 +2084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:Q2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,9 +2100,16 @@
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="17" width="20.7109375" customWidth="1"/>
+    <col min="18" max="18" width="39.28515625" customWidth="1"/>
+    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2124,8 +2161,20 @@
       <c r="Q1" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>549</v>
+      </c>
+      <c r="S1" t="s">
+        <v>550</v>
+      </c>
+      <c r="T1" t="s">
+        <v>551</v>
+      </c>
+      <c r="U1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
@@ -2176,6 +2225,15 @@
       </c>
       <c r="Q2" t="s">
         <v>509</v>
+      </c>
+      <c r="R2" t="s">
+        <v>440</v>
+      </c>
+      <c r="T2" t="s">
+        <v>553</v>
+      </c>
+      <c r="U2" t="s">
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -2184,6 +2242,43 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -2295,7 +2390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -2373,7 +2468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2413,7 +2508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB10"/>
   <sheetViews>
@@ -2798,7 +2893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
@@ -2950,7 +3045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -3071,7 +3166,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -3153,7 +3248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -3258,7 +3353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -3346,7 +3441,63 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D1" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>546</v>
+      </c>
+      <c r="B2" t="s">
+        <v>462</v>
+      </c>
+      <c r="C2" t="s">
+        <v>547</v>
+      </c>
+      <c r="D2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -3453,38 +3604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -3592,7 +3712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -3673,7 +3793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -3812,7 +3932,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
@@ -3994,7 +4114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -4029,7 +4149,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -4132,7 +4252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -4239,7 +4359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -4339,7 +4459,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -4439,7 +4559,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -4476,7 +4627,814 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D1" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B2" t="s">
+        <v>462</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="E2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S5"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F1" t="s">
+        <v>402</v>
+      </c>
+      <c r="G1" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1" t="s">
+        <v>405</v>
+      </c>
+      <c r="J1" t="s">
+        <v>406</v>
+      </c>
+      <c r="K1" t="s">
+        <v>399</v>
+      </c>
+      <c r="L1" t="s">
+        <v>400</v>
+      </c>
+      <c r="M1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O1" t="s">
+        <v>401</v>
+      </c>
+      <c r="P1" t="s">
+        <v>465</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>466</v>
+      </c>
+      <c r="R1" t="s">
+        <v>467</v>
+      </c>
+      <c r="S1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C2" t="s">
+        <v>470</v>
+      </c>
+      <c r="D2" t="s">
+        <v>471</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="F2" t="s">
+        <v>472</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" t="s">
+        <v>414</v>
+      </c>
+      <c r="M2" t="s">
+        <v>414</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>477</v>
+      </c>
+      <c r="R2" t="s">
+        <v>478</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="S2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" t="s">
+        <v>483</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>437</v>
+      </c>
+      <c r="H1" t="s">
+        <v>484</v>
+      </c>
+      <c r="I1" t="s">
+        <v>485</v>
+      </c>
+      <c r="J1" t="s">
+        <v>486</v>
+      </c>
+      <c r="K1" t="s">
+        <v>487</v>
+      </c>
+      <c r="L1" t="s">
+        <v>543</v>
+      </c>
+      <c r="M1" t="s">
+        <v>544</v>
+      </c>
+      <c r="N1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="C2" t="s">
+        <v>490</v>
+      </c>
+      <c r="D2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E2" t="s">
+        <v>414</v>
+      </c>
+      <c r="F2" t="s">
+        <v>414</v>
+      </c>
+      <c r="G2">
+        <v>123456</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="J2">
+        <v>123</v>
+      </c>
+      <c r="K2" t="s">
+        <v>488</v>
+      </c>
+      <c r="L2" t="s">
+        <v>462</v>
+      </c>
+      <c r="M2" t="s">
+        <v>463</v>
+      </c>
+      <c r="N2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>545</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H4" s="3" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H5" s="3" t="s">
+        <v>492</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.28515625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E1" t="s">
+        <v>431</v>
+      </c>
+      <c r="F1" t="s">
+        <v>432</v>
+      </c>
+      <c r="G1" t="s">
+        <v>433</v>
+      </c>
+      <c r="H1" t="s">
+        <v>434</v>
+      </c>
+      <c r="I1" t="s">
+        <v>435</v>
+      </c>
+      <c r="J1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" t="s">
+        <v>436</v>
+      </c>
+      <c r="L1" t="s">
+        <v>437</v>
+      </c>
+      <c r="M1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>44713</v>
+      </c>
+      <c r="B2" s="7">
+        <v>44774</v>
+      </c>
+      <c r="C2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="F2" t="s">
+        <v>438</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="H2">
+        <v>123</v>
+      </c>
+      <c r="I2" t="s">
+        <v>444</v>
+      </c>
+      <c r="J2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="L2">
+        <v>123456</v>
+      </c>
+      <c r="M2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="26.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1" t="s">
+        <v>403</v>
+      </c>
+      <c r="E1" t="s">
+        <v>404</v>
+      </c>
+      <c r="F1" t="s">
+        <v>405</v>
+      </c>
+      <c r="G1" t="s">
+        <v>406</v>
+      </c>
+      <c r="H1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B2" t="s">
+        <v>511</v>
+      </c>
+      <c r="C2" t="s">
+        <v>512</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>513</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B2" t="s">
+        <v>519</v>
+      </c>
+      <c r="C2" t="s">
+        <v>520</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>521</v>
+      </c>
+      <c r="B3" t="s">
+        <v>522</v>
+      </c>
+      <c r="C3" t="s">
+        <v>523</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>524</v>
+      </c>
+      <c r="B4" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>526</v>
+      </c>
+      <c r="B5" t="s">
+        <v>519</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1" t="s">
+        <v>529</v>
+      </c>
+      <c r="D1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
+        <v>396</v>
+      </c>
+      <c r="F1" t="s">
+        <v>397</v>
+      </c>
+      <c r="G1" t="s">
+        <v>398</v>
+      </c>
+      <c r="H1" t="s">
+        <v>399</v>
+      </c>
+      <c r="I1" t="s">
+        <v>400</v>
+      </c>
+      <c r="J1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" t="s">
+        <v>152</v>
+      </c>
+      <c r="L1" t="s">
+        <v>401</v>
+      </c>
+      <c r="M1" t="s">
+        <v>402</v>
+      </c>
+      <c r="N1" t="s">
+        <v>403</v>
+      </c>
+      <c r="O1" t="s">
+        <v>404</v>
+      </c>
+      <c r="P1" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>530</v>
+      </c>
+      <c r="B2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C2" t="s">
+        <v>532</v>
+      </c>
+      <c r="D2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" t="s">
+        <v>533</v>
+      </c>
+      <c r="F2" t="s">
+        <v>534</v>
+      </c>
+      <c r="G2" t="s">
+        <v>512</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" t="s">
+        <v>414</v>
+      </c>
+      <c r="J2" t="s">
+        <v>414</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="M2" t="s">
+        <v>535</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N3" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -4598,707 +5556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>453</v>
-      </c>
-      <c r="B1" t="s">
-        <v>454</v>
-      </c>
-      <c r="C1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>456</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>443</v>
-      </c>
-      <c r="B1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" t="s">
-        <v>458</v>
-      </c>
-      <c r="D1" t="s">
-        <v>459</v>
-      </c>
-      <c r="E1" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>461</v>
-      </c>
-      <c r="B2" t="s">
-        <v>462</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="E2" t="s">
-        <v>463</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
-  <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>464</v>
-      </c>
-      <c r="B1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C1" t="s">
-        <v>396</v>
-      </c>
-      <c r="D1" t="s">
-        <v>397</v>
-      </c>
-      <c r="E1" t="s">
-        <v>398</v>
-      </c>
-      <c r="F1" t="s">
-        <v>402</v>
-      </c>
-      <c r="G1" t="s">
-        <v>403</v>
-      </c>
-      <c r="H1" t="s">
-        <v>404</v>
-      </c>
-      <c r="I1" t="s">
-        <v>405</v>
-      </c>
-      <c r="J1" t="s">
-        <v>406</v>
-      </c>
-      <c r="K1" t="s">
-        <v>399</v>
-      </c>
-      <c r="L1" t="s">
-        <v>400</v>
-      </c>
-      <c r="M1" t="s">
-        <v>104</v>
-      </c>
-      <c r="N1" t="s">
-        <v>152</v>
-      </c>
-      <c r="O1" t="s">
-        <v>401</v>
-      </c>
-      <c r="P1" t="s">
-        <v>465</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>466</v>
-      </c>
-      <c r="R1" t="s">
-        <v>467</v>
-      </c>
-      <c r="S1" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" t="s">
-        <v>469</v>
-      </c>
-      <c r="C2" t="s">
-        <v>470</v>
-      </c>
-      <c r="D2" t="s">
-        <v>471</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>413</v>
-      </c>
-      <c r="F2" t="s">
-        <v>472</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>475</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="L2" t="s">
-        <v>414</v>
-      </c>
-      <c r="M2" t="s">
-        <v>414</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>477</v>
-      </c>
-      <c r="R2" t="s">
-        <v>478</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="S2" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>482</v>
-      </c>
-      <c r="B1" t="s">
-        <v>436</v>
-      </c>
-      <c r="C1" t="s">
-        <v>398</v>
-      </c>
-      <c r="D1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E1" t="s">
-        <v>483</v>
-      </c>
-      <c r="F1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" t="s">
-        <v>437</v>
-      </c>
-      <c r="H1" t="s">
-        <v>484</v>
-      </c>
-      <c r="I1" t="s">
-        <v>485</v>
-      </c>
-      <c r="J1" t="s">
-        <v>486</v>
-      </c>
-      <c r="K1" t="s">
-        <v>487</v>
-      </c>
-      <c r="L1" t="s">
-        <v>543</v>
-      </c>
-      <c r="M1" t="s">
-        <v>544</v>
-      </c>
-      <c r="N1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>489</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="C2" t="s">
-        <v>490</v>
-      </c>
-      <c r="D2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E2" t="s">
-        <v>414</v>
-      </c>
-      <c r="F2" t="s">
-        <v>414</v>
-      </c>
-      <c r="G2">
-        <v>123456</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>493</v>
-      </c>
-      <c r="J2">
-        <v>123</v>
-      </c>
-      <c r="K2" t="s">
-        <v>488</v>
-      </c>
-      <c r="L2" t="s">
-        <v>462</v>
-      </c>
-      <c r="M2" t="s">
-        <v>463</v>
-      </c>
-      <c r="N2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H3" t="s">
-        <v>545</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H4" s="3" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H5" s="3" t="s">
-        <v>492</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>396</v>
-      </c>
-      <c r="B1" t="s">
-        <v>397</v>
-      </c>
-      <c r="C1" t="s">
-        <v>398</v>
-      </c>
-      <c r="D1" t="s">
-        <v>403</v>
-      </c>
-      <c r="E1" t="s">
-        <v>404</v>
-      </c>
-      <c r="F1" t="s">
-        <v>405</v>
-      </c>
-      <c r="G1" t="s">
-        <v>406</v>
-      </c>
-      <c r="H1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>510</v>
-      </c>
-      <c r="B2" t="s">
-        <v>511</v>
-      </c>
-      <c r="C2" t="s">
-        <v>512</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>513</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>514</v>
-      </c>
-      <c r="B1" t="s">
-        <v>515</v>
-      </c>
-      <c r="C1" t="s">
-        <v>516</v>
-      </c>
-      <c r="D1" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>518</v>
-      </c>
-      <c r="B2" t="s">
-        <v>519</v>
-      </c>
-      <c r="C2" t="s">
-        <v>520</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>521</v>
-      </c>
-      <c r="B3" t="s">
-        <v>522</v>
-      </c>
-      <c r="C3" t="s">
-        <v>523</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>524</v>
-      </c>
-      <c r="B4" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>526</v>
-      </c>
-      <c r="B5" t="s">
-        <v>519</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>527</v>
-      </c>
-      <c r="B1" t="s">
-        <v>528</v>
-      </c>
-      <c r="C1" t="s">
-        <v>529</v>
-      </c>
-      <c r="D1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E1" t="s">
-        <v>396</v>
-      </c>
-      <c r="F1" t="s">
-        <v>397</v>
-      </c>
-      <c r="G1" t="s">
-        <v>398</v>
-      </c>
-      <c r="H1" t="s">
-        <v>399</v>
-      </c>
-      <c r="I1" t="s">
-        <v>400</v>
-      </c>
-      <c r="J1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" t="s">
-        <v>152</v>
-      </c>
-      <c r="L1" t="s">
-        <v>401</v>
-      </c>
-      <c r="M1" t="s">
-        <v>402</v>
-      </c>
-      <c r="N1" t="s">
-        <v>403</v>
-      </c>
-      <c r="O1" t="s">
-        <v>404</v>
-      </c>
-      <c r="P1" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>530</v>
-      </c>
-      <c r="B2" t="s">
-        <v>531</v>
-      </c>
-      <c r="C2" t="s">
-        <v>532</v>
-      </c>
-      <c r="D2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" t="s">
-        <v>533</v>
-      </c>
-      <c r="F2" t="s">
-        <v>534</v>
-      </c>
-      <c r="G2" t="s">
-        <v>512</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="I2" t="s">
-        <v>414</v>
-      </c>
-      <c r="J2" t="s">
-        <v>414</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="M2" t="s">
-        <v>535</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N3" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>424</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -5371,7 +5629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -5420,7 +5678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -5508,7 +5766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -5552,7 +5810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -5657,7 +5915,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -5690,41 +5948,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>